<commit_message>
- Endra fargekoding for betre universell utforming - La til kolonne for progresjonsvariabel, for å kunne fargekode tidsvariabel - Endra oppsett for å sette programvariablar - Rydda kommentarar
</commit_message>
<xml_diff>
--- a/malfiler/Studiebarometeret_2023_vars.xlsx
+++ b/malfiler/Studiebarometeret_2023_vars.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{C138724C-99B5-4021-A7A5-493A6B263C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A20342EB-6410-4E27-88C3-844AE307A26C}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{C138724C-99B5-4021-A7A5-493A6B263C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A927274D-A33C-45D1-A814-E1117E226F7D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
   <si>
     <t>Variabel</t>
   </si>
@@ -234,9 +234,6 @@
     <t>Betalt arbeid</t>
   </si>
   <si>
-    <t>Studiebarometeret 2021</t>
-  </si>
-  <si>
     <t>I hvilken grad er du enig i de følgende påstandene</t>
   </si>
   <si>
@@ -391,6 +388,21 @@
   </si>
   <si>
     <t>overord_altialt_13</t>
+  </si>
+  <si>
+    <t>Studiebarometeret 2022</t>
+  </si>
+  <si>
+    <t>Andel heltid</t>
+  </si>
+  <si>
+    <t>progresjon</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>prosent</t>
   </si>
 </sst>
 </file>
@@ -756,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E65" sqref="A60:E65"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +783,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -787,10 +799,13 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -799,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -808,20 +823,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -833,144 +848,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" s="2" t="b">
         <v>0</v>
@@ -981,7 +996,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17"/>
       <c r="E17" s="2" t="b">
@@ -995,7 +1010,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="2" t="b">
         <v>0</v>
@@ -1008,7 +1023,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>0</v>
@@ -1021,7 +1036,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>0</v>
@@ -1034,7 +1049,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="2" t="b">
         <v>0</v>
@@ -1047,7 +1062,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="b">
         <v>0</v>
@@ -1072,7 +1087,7 @@
         <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>0</v>
@@ -1085,7 +1100,7 @@
         <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E25" s="2" t="b">
         <v>0</v>
@@ -1098,7 +1113,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>0</v>
@@ -1111,7 +1126,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>0</v>
@@ -1124,7 +1139,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>0</v>
@@ -1135,7 +1150,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29"/>
       <c r="E29" s="2" t="b">
@@ -1149,7 +1164,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" s="2" t="b">
         <v>0</v>
@@ -1162,7 +1177,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="2" t="b">
         <v>0</v>
@@ -1175,7 +1190,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>0</v>
@@ -1188,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="2" t="b">
         <v>0</v>
@@ -1201,7 +1216,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="2" t="b">
         <v>0</v>
@@ -1226,7 +1241,7 @@
         <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E36" s="2" t="b">
         <v>0</v>
@@ -1239,7 +1254,7 @@
         <v>40</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="2" t="b">
         <v>0</v>
@@ -1252,7 +1267,7 @@
         <v>41</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E38" s="2" t="b">
         <v>0</v>
@@ -1265,7 +1280,7 @@
         <v>42</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E39" s="2" t="b">
         <v>0</v>
@@ -1276,7 +1291,7 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40"/>
       <c r="E40" s="2" t="b">
@@ -1292,7 +1307,7 @@
         <v>44</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E41" s="2" t="b">
         <v>0</v>
@@ -1317,7 +1332,7 @@
         <v>47</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E43" s="2" t="b">
         <v>0</v>
@@ -1330,7 +1345,7 @@
         <v>48</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E44" s="2" t="b">
         <v>0</v>
@@ -1343,7 +1358,7 @@
         <v>49</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E45" s="2" t="b">
         <v>0</v>
@@ -1356,7 +1371,7 @@
         <v>50</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E46" s="2" t="b">
         <v>0</v>
@@ -1369,7 +1384,7 @@
         <v>51</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E47" s="2" t="b">
         <v>0</v>
@@ -1387,85 +1402,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49" t="s">
         <v>54</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50" t="s">
         <v>55</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51" t="s">
         <v>56</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52" t="s">
         <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E52" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53" t="s">
         <v>58</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E53" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54" t="s">
         <v>59</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E54" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1477,54 +1492,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56" t="s">
         <v>62</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E56" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57" t="s">
         <v>63</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E57" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58" t="s">
         <v>64</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E58" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>65</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E59" s="2" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- La til formatering av "Sum tid studier" i tre nivå: under landssnitt, over minimum forventa tid (1500 t/år) og over maksimum forventa tid (1800 t/år)
</commit_message>
<xml_diff>
--- a/malfiler/Studiebarometeret_2023_vars.xlsx
+++ b/malfiler/Studiebarometeret_2023_vars.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{C138724C-99B5-4021-A7A5-493A6B263C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A927274D-A33C-45D1-A814-E1117E226F7D}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{C138724C-99B5-4021-A7A5-493A6B263C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFFE33C6-1CD9-4A4E-B527-7E57B3527469}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1550,7 @@
         <v>120</v>
       </c>
       <c r="E60" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>122</v>

</xml_diff>